<commit_message>
study(23_Project): main project design
</commit_message>
<xml_diff>
--- a/23_Project/Main_Project/project_design/vegitable_market_project_design.xlsx
+++ b/23_Project/Main_Project/project_design/vegitable_market_project_design.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Study\Develop\Codecamp_Backend\23_Project\Main_Project\project_design\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0B84290F-9F72-4BBE-95D2-F6BDFDF87172}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E84256D8-2C56-460F-8454-8D3F7DC02E20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="19095" yWindow="0" windowWidth="19410" windowHeight="15585" xr2:uid="{C60A6398-7BE2-4883-A906-74D347AFAF11}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="63">
   <si>
     <t>페이지</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -111,10 +111,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>로그인 에러 창</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>확인되는 가입 정보가 없습니다. 회원가입을 진행해주세요.</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -268,6 +264,18 @@
   </si>
   <si>
     <t>팔래요 메뉴</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>로그인 없이 둘러보기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>비밀번호가 일치하지 않습니다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>로그인 에러 알림창</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -647,10 +655,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{430947C9-B8B0-4DE3-877D-B69BC3F0167A}">
-  <dimension ref="A1:G62"/>
+  <dimension ref="A1:G64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="C53" sqref="C53"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="G42" sqref="G42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -734,101 +742,101 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G5" s="3"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
-      <c r="B6" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>9</v>
-      </c>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
+      <c r="B7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
-      <c r="B8" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>49</v>
-      </c>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
       <c r="G8" s="1"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="1"/>
-      <c r="B9" s="3"/>
+      <c r="B9" s="3" t="s">
+        <v>24</v>
+      </c>
       <c r="C9" s="1" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>19</v>
       </c>
       <c r="E9" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F9" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="F9" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="G9" s="1"/>
+      <c r="G9" s="3"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="1"/>
       <c r="B10" s="3"/>
       <c r="C10" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E10" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="D10" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>9</v>
-      </c>
       <c r="F10" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G10" s="1"/>
+        <v>49</v>
+      </c>
+      <c r="G10" s="3"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="1"/>
       <c r="B11" s="3"/>
       <c r="C11" s="1" t="s">
-        <v>17</v>
+        <v>46</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>20</v>
@@ -839,30 +847,30 @@
       <c r="F11" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G11" s="1"/>
+      <c r="G11" s="3"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="1"/>
       <c r="B12" s="3"/>
       <c r="C12" s="1" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>48</v>
+        <v>9</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G12" s="1"/>
+      <c r="G12" s="3"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="1"/>
       <c r="B13" s="3"/>
       <c r="C13" s="1" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>8</v>
@@ -873,24 +881,30 @@
       <c r="F13" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G13" s="1"/>
+      <c r="G13" s="3"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="1"/>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
-      <c r="G14" s="1"/>
+      <c r="B14" s="3"/>
+      <c r="C14" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G14" s="3"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="1"/>
-      <c r="B15" s="3" t="s">
-        <v>21</v>
-      </c>
+      <c r="B15" s="3"/>
       <c r="C15" s="1" t="s">
-        <v>22</v>
+        <v>61</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>20</v>
@@ -901,33 +915,27 @@
       <c r="F15" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G15" s="1"/>
+      <c r="G15" s="3"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="1"/>
-      <c r="B16" s="3"/>
-      <c r="C16" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>9</v>
-      </c>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
       <c r="G16" s="1"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="1"/>
-      <c r="B17" s="3"/>
+      <c r="B17" s="3" t="s">
+        <v>62</v>
+      </c>
       <c r="C17" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>9</v>
@@ -935,154 +943,154 @@
       <c r="F17" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G17" s="1"/>
+      <c r="G17" s="3"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="1"/>
-      <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
-      <c r="F18" s="1"/>
-      <c r="G18" s="1"/>
+      <c r="B18" s="3"/>
+      <c r="C18" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G18" s="3"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="1"/>
-      <c r="B19" s="3" t="s">
-        <v>26</v>
-      </c>
+      <c r="B19" s="3"/>
       <c r="C19" s="1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>46</v>
+        <v>9</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="G19" s="1"/>
+        <v>9</v>
+      </c>
+      <c r="G19" s="3"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" s="1"/>
-      <c r="B20" s="3"/>
-      <c r="C20" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>51</v>
-      </c>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
       <c r="G20" s="1"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" s="1"/>
-      <c r="B21" s="3"/>
+      <c r="B21" s="3" t="s">
+        <v>25</v>
+      </c>
       <c r="C21" s="1" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="G21" s="1"/>
+        <v>45</v>
+      </c>
+      <c r="G21" s="3"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" s="1"/>
       <c r="B22" s="3"/>
       <c r="C22" s="1" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>19</v>
       </c>
       <c r="E22" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F22" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="F22" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="G22" s="1"/>
+      <c r="G22" s="3"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" s="1"/>
       <c r="B23" s="3"/>
       <c r="C23" s="1" t="s">
-        <v>29</v>
+        <v>12</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>19</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="G23" s="1"/>
+        <v>49</v>
+      </c>
+      <c r="G23" s="3"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" s="1"/>
       <c r="B24" s="3"/>
       <c r="C24" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G24" s="1"/>
+        <v>50</v>
+      </c>
+      <c r="G24" s="3"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" s="1"/>
       <c r="B25" s="3"/>
       <c r="C25" s="1" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G25" s="1"/>
+        <v>51</v>
+      </c>
+      <c r="G25" s="3"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" s="1"/>
       <c r="B26" s="3"/>
       <c r="C26" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F26" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G26" s="1"/>
+      <c r="G26" s="3"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" s="1"/>
@@ -1091,41 +1099,41 @@
         <v>32</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>9</v>
+        <v>47</v>
       </c>
       <c r="F27" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G27" s="1"/>
+      <c r="G27" s="3"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" s="1"/>
       <c r="B28" s="3"/>
       <c r="C28" s="1" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>35</v>
+        <v>19</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F28" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G28" s="1"/>
+      <c r="G28" s="3"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" s="1"/>
       <c r="B29" s="3"/>
       <c r="C29" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="E29" s="1" t="s">
         <v>9</v>
@@ -1133,7 +1141,7 @@
       <c r="F29" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G29" s="1"/>
+      <c r="G29" s="3"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" s="1"/>
@@ -1142,21 +1150,21 @@
         <v>36</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F30" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G30" s="1"/>
+      <c r="G30" s="3"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" s="1"/>
       <c r="B31" s="3"/>
       <c r="C31" s="1" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="D31" s="1" t="s">
         <v>8</v>
@@ -1167,33 +1175,33 @@
       <c r="F31" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G31" s="1"/>
+      <c r="G31" s="3"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" s="1"/>
       <c r="B32" s="3"/>
       <c r="C32" s="1" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F32" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G32" s="1"/>
+      <c r="G32" s="3"/>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" s="1"/>
       <c r="B33" s="3"/>
       <c r="C33" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="E33" s="1" t="s">
         <v>9</v>
@@ -1201,98 +1209,112 @@
       <c r="F33" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G33" s="1"/>
+      <c r="G33" s="3"/>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34" s="1"/>
       <c r="B34" s="3"/>
       <c r="C34" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>8</v>
+        <v>34</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F34" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G34" s="1"/>
+      <c r="G34" s="3"/>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35" s="1"/>
-      <c r="B35" s="1"/>
-      <c r="C35" s="1"/>
-      <c r="D35" s="1"/>
-      <c r="E35" s="1"/>
-      <c r="F35" s="1"/>
-      <c r="G35" s="1"/>
+      <c r="B35" s="3"/>
+      <c r="C35" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G35" s="3"/>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36" s="1"/>
-      <c r="B36" s="3" t="s">
-        <v>39</v>
-      </c>
+      <c r="B36" s="3"/>
       <c r="C36" s="1" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="F36" s="1"/>
-      <c r="G36" s="1"/>
+        <v>47</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G36" s="3"/>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37" s="1"/>
-      <c r="B37" s="3"/>
-      <c r="C37" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="D37" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E37" s="1" t="s">
-        <v>9</v>
-      </c>
+      <c r="B37" s="1"/>
+      <c r="C37" s="1"/>
+      <c r="D37" s="1"/>
+      <c r="E37" s="1"/>
       <c r="F37" s="1"/>
       <c r="G37" s="1"/>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38" s="1"/>
-      <c r="B38" s="3"/>
+      <c r="B38" s="3" t="s">
+        <v>38</v>
+      </c>
       <c r="C38" s="1" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>44</v>
+        <v>20</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F38" s="1"/>
       <c r="G38" s="1"/>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39" s="1"/>
-      <c r="B39" s="1"/>
-      <c r="C39" s="1"/>
-      <c r="D39" s="1"/>
-      <c r="E39" s="1"/>
+      <c r="B39" s="3"/>
+      <c r="C39" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="F39" s="1"/>
       <c r="G39" s="1"/>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A40" s="1"/>
-      <c r="B40" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="C40" s="1"/>
-      <c r="D40" s="1"/>
-      <c r="E40" s="1"/>
+      <c r="B40" s="3"/>
+      <c r="C40" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>47</v>
+      </c>
       <c r="F40" s="1"/>
       <c r="G40" s="1"/>
     </row>
@@ -1308,7 +1330,7 @@
     <row r="42" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A42" s="1"/>
       <c r="B42" s="1" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="C42" s="1"/>
       <c r="D42" s="1"/>
@@ -1328,7 +1350,7 @@
     <row r="44" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A44" s="1"/>
       <c r="B44" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C44" s="1"/>
       <c r="D44" s="1"/>
@@ -1348,7 +1370,7 @@
     <row r="46" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A46" s="1"/>
       <c r="B46" s="1" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="C46" s="1"/>
       <c r="D46" s="1"/>
@@ -1368,7 +1390,7 @@
     <row r="48" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A48" s="1"/>
       <c r="B48" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C48" s="1"/>
       <c r="D48" s="1"/>
@@ -1388,7 +1410,7 @@
     <row r="50" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A50" s="1"/>
       <c r="B50" s="1" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="C50" s="1"/>
       <c r="D50" s="1"/>
@@ -1408,7 +1430,7 @@
     <row r="52" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A52" s="1"/>
       <c r="B52" s="1" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="C52" s="1"/>
       <c r="D52" s="1"/>
@@ -1428,7 +1450,7 @@
     <row r="54" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A54" s="1"/>
       <c r="B54" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C54" s="1"/>
       <c r="D54" s="1"/>
@@ -1447,7 +1469,9 @@
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A56" s="1"/>
-      <c r="B56" s="1"/>
+      <c r="B56" s="1" t="s">
+        <v>56</v>
+      </c>
       <c r="C56" s="1"/>
       <c r="D56" s="1"/>
       <c r="E56" s="1"/>
@@ -1508,14 +1532,35 @@
       <c r="F62" s="1"/>
       <c r="G62" s="1"/>
     </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A63" s="1"/>
+      <c r="B63" s="1"/>
+      <c r="C63" s="1"/>
+      <c r="D63" s="1"/>
+      <c r="E63" s="1"/>
+      <c r="F63" s="1"/>
+      <c r="G63" s="1"/>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A64" s="1"/>
+      <c r="B64" s="1"/>
+      <c r="C64" s="1"/>
+      <c r="D64" s="1"/>
+      <c r="E64" s="1"/>
+      <c r="F64" s="1"/>
+      <c r="G64" s="1"/>
+    </row>
   </sheetData>
-  <mergeCells count="6">
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="G3:G4"/>
-    <mergeCell ref="B8:B13"/>
-    <mergeCell ref="B15:B17"/>
-    <mergeCell ref="B19:B34"/>
-    <mergeCell ref="B36:B38"/>
+  <mergeCells count="9">
+    <mergeCell ref="B38:B40"/>
+    <mergeCell ref="G9:G15"/>
+    <mergeCell ref="G17:G19"/>
+    <mergeCell ref="G21:G36"/>
+    <mergeCell ref="B3:B5"/>
+    <mergeCell ref="G3:G5"/>
+    <mergeCell ref="B9:B15"/>
+    <mergeCell ref="B17:B19"/>
+    <mergeCell ref="B21:B36"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>